<commit_message>
New point maps for the new experiments
</commit_message>
<xml_diff>
--- a/AD-EYE/Experiments/Test_World_1/Simulation/TAconstant1.xlsx
+++ b/AD-EYE/Experiments/Test_World_1/Simulation/TAconstant1.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Radhika\Desktop\RUT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adeye\AD-EYE_Core\AD-EYE\Experiments\Test_World_1\Simulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB7628A-41FA-40C5-89DE-9A288D463DEA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="5085" windowHeight="2985"/>
+    <workbookView xWindow="30870" yWindow="2430" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -119,7 +120,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -430,11 +431,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -479,7 +480,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -487,7 +488,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
New worlds with actors and update in the TA.m
</commit_message>
<xml_diff>
--- a/AD-EYE/Experiments/Test_World_1/Simulation/TAconstant1.xlsx
+++ b/AD-EYE/Experiments/Test_World_1/Simulation/TAconstant1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adeye\AD-EYE_Core\AD-EYE\Experiments\Test_World_1\Simulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB7628A-41FA-40C5-89DE-9A288D463DEA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2442ADC6-6E5D-4DD5-B6BF-C2EE0BFAF349}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30870" yWindow="2430" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30270" yWindow="1470" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>BlockName</t>
   </si>
@@ -73,9 +73,6 @@
   </si>
   <si>
     <t>BMW_X5_SUV_1/GoalOrientX</t>
-  </si>
-  <si>
-    <t>0.707</t>
   </si>
   <si>
     <t>BMW_X5_SUV_1/GoalOrientY</t>
@@ -150,8 +147,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -559,13 +557,13 @@
       <c r="A15" t="s">
         <v>15</v>
       </c>
-      <c r="B15" t="s">
-        <v>16</v>
+      <c r="B15" s="1">
+        <v>0.70699999999999996</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -573,7 +571,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -581,15 +579,15 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0.70699999999999996</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19">
         <v>10</v>
@@ -597,7 +595,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B20">
         <v>2</v>
@@ -605,7 +603,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21">
         <v>100</v>
@@ -613,7 +611,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22">
         <v>100</v>
@@ -621,7 +619,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23">
         <v>100</v>
@@ -629,7 +627,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B24">
         <v>100</v>
@@ -637,7 +635,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B25">
         <v>100</v>
@@ -645,7 +643,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B26">
         <v>100</v>
@@ -653,7 +651,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B27">
         <v>100</v>
@@ -661,7 +659,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B28">
         <v>10</v>

</xml_diff>